<commit_message>
Ejercicio 2 (QAA-02) API TestAutomatizados
Se actualiza TestCase se elimina la prueba N°8
</commit_message>
<xml_diff>
--- a/Ejercicio 2 (QAA-02) API TestAutomatizados.xlsx
+++ b/Ejercicio 2 (QAA-02) API TestAutomatizados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRINIDAD\Desktop\CleverIT\Solución_Daniel_Rojas_Mesias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cursoGit\GIT\clverIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA73B6B9-970F-4F38-8FA0-00B68E003220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02BB6FE-6DFF-4495-84B9-27F7CE7B822D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC1B522D-3CF4-4921-9D18-B874CCAD5142}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BC1B522D-3CF4-4921-9D18-B874CCAD5142}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="44">
   <si>
     <t>CP</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>CP8</t>
-  </si>
-  <si>
-    <t>Validar que nos trae un Users especifico</t>
   </si>
   <si>
     <t xml:space="preserve">Host =  https://jsonplaceholder.typicode.com                                Endpoint = Albums                                                                                                                      </t>
@@ -662,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D429E79F-2092-43E2-91B6-6F1BA6FF248F}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.33203125" defaultRowHeight="52.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -711,7 +708,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>26</v>
@@ -734,7 +731,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>23</v>
@@ -757,7 +754,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>27</v>
@@ -780,7 +777,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>22</v>
@@ -803,7 +800,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>25</v>
@@ -826,7 +823,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>29</v>
@@ -849,36 +846,13 @@
         <v>16</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -931,10 +905,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>26</v>
@@ -954,10 +928,10 @@
         <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>23</v>
@@ -977,10 +951,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>27</v>
@@ -1000,10 +974,10 @@
         <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>22</v>
@@ -1023,10 +997,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>25</v>
@@ -1046,10 +1020,10 @@
         <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>29</v>
@@ -1069,10 +1043,10 @@
         <v>31</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>30</v>
@@ -1089,19 +1063,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1156,10 +1130,10 @@
         <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>26</v>
@@ -1179,10 +1153,10 @@
         <v>20</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>23</v>
@@ -1202,10 +1176,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>27</v>
@@ -1225,10 +1199,10 @@
         <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>22</v>
@@ -1248,10 +1222,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>25</v>
@@ -1271,10 +1245,10 @@
         <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>29</v>
@@ -1294,10 +1268,10 @@
         <v>31</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>30</v>
@@ -1314,19 +1288,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>